<commit_message>
Ultimate fix on backend
</commit_message>
<xml_diff>
--- a/media/output/result/sepsis_cases_1_complex_evaluation_edit_distance_lib.xlsx
+++ b/media/output/result/sepsis_cases_1_complex_evaluation_edit_distance_lib.xlsx
@@ -476,11 +476,11 @@
         <v>151</v>
       </c>
       <c r="C2" t="n">
+        <v>135</v>
+      </c>
+      <c r="D2" t="n">
         <v>16</v>
       </c>
-      <c r="D2" t="n">
-        <v>135</v>
-      </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
@@ -488,13 +488,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="3">
@@ -505,11 +505,11 @@
         <v>151</v>
       </c>
       <c r="C3" t="n">
+        <v>135</v>
+      </c>
+      <c r="D3" t="n">
         <v>16</v>
       </c>
-      <c r="D3" t="n">
-        <v>135</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
@@ -517,13 +517,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="4">
@@ -534,11 +534,11 @@
         <v>151</v>
       </c>
       <c r="C4" t="n">
+        <v>135</v>
+      </c>
+      <c r="D4" t="n">
         <v>16</v>
       </c>
-      <c r="D4" t="n">
-        <v>135</v>
-      </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
@@ -546,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="5">
@@ -563,11 +563,11 @@
         <v>151</v>
       </c>
       <c r="C5" t="n">
+        <v>135</v>
+      </c>
+      <c r="D5" t="n">
         <v>16</v>
       </c>
-      <c r="D5" t="n">
-        <v>135</v>
-      </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
@@ -575,13 +575,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="6">
@@ -592,11 +592,11 @@
         <v>151</v>
       </c>
       <c r="C6" t="n">
+        <v>135</v>
+      </c>
+      <c r="D6" t="n">
         <v>16</v>
       </c>
-      <c r="D6" t="n">
-        <v>135</v>
-      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
@@ -604,13 +604,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="7">
@@ -621,11 +621,11 @@
         <v>151</v>
       </c>
       <c r="C7" t="n">
+        <v>135</v>
+      </c>
+      <c r="D7" t="n">
         <v>16</v>
       </c>
-      <c r="D7" t="n">
-        <v>135</v>
-      </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
@@ -633,13 +633,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="8">
@@ -650,11 +650,11 @@
         <v>151</v>
       </c>
       <c r="C8" t="n">
+        <v>135</v>
+      </c>
+      <c r="D8" t="n">
         <v>16</v>
       </c>
-      <c r="D8" t="n">
-        <v>135</v>
-      </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
@@ -662,13 +662,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="9">
@@ -679,11 +679,11 @@
         <v>151</v>
       </c>
       <c r="C9" t="n">
+        <v>135</v>
+      </c>
+      <c r="D9" t="n">
         <v>16</v>
       </c>
-      <c r="D9" t="n">
-        <v>135</v>
-      </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
@@ -691,13 +691,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1059602649006623</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1916167664670659</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="10">
@@ -708,11 +708,11 @@
         <v>148</v>
       </c>
       <c r="C10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D10" t="n">
         <v>16</v>
       </c>
-      <c r="D10" t="n">
-        <v>132</v>
-      </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
@@ -720,13 +720,13 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1081081081081081</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1951219512195122</v>
+        <v>0.9428571428571428</v>
       </c>
     </row>
     <row r="11">
@@ -737,11 +737,11 @@
         <v>146</v>
       </c>
       <c r="C11" t="n">
+        <v>130</v>
+      </c>
+      <c r="D11" t="n">
         <v>16</v>
       </c>
-      <c r="D11" t="n">
-        <v>130</v>
-      </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
@@ -749,13 +749,13 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1095890410958904</v>
+        <v>0.8904109589041096</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1975308641975309</v>
+        <v>0.9420289855072463</v>
       </c>
     </row>
     <row r="12">
@@ -766,11 +766,11 @@
         <v>135</v>
       </c>
       <c r="C12" t="n">
+        <v>121</v>
+      </c>
+      <c r="D12" t="n">
         <v>14</v>
       </c>
-      <c r="D12" t="n">
-        <v>121</v>
-      </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
@@ -778,13 +778,13 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1037037037037037</v>
+        <v>0.8962962962962963</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1879194630872483</v>
+        <v>0.9453124999999999</v>
       </c>
     </row>
     <row r="13">
@@ -795,11 +795,11 @@
         <v>121</v>
       </c>
       <c r="C13" t="n">
+        <v>109</v>
+      </c>
+      <c r="D13" t="n">
         <v>12</v>
       </c>
-      <c r="D13" t="n">
-        <v>109</v>
-      </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
@@ -807,13 +807,13 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.09917355371900827</v>
+        <v>0.9008264462809917</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1804511278195489</v>
+        <v>0.9478260869565218</v>
       </c>
     </row>
     <row r="14">
@@ -824,11 +824,11 @@
         <v>102</v>
       </c>
       <c r="C14" t="n">
+        <v>93</v>
+      </c>
+      <c r="D14" t="n">
         <v>9</v>
       </c>
-      <c r="D14" t="n">
-        <v>93</v>
-      </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
@@ -836,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.08823529411764706</v>
+        <v>0.9117647058823529</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1621621621621622</v>
+        <v>0.9538461538461539</v>
       </c>
     </row>
     <row r="15">
@@ -853,11 +853,11 @@
         <v>86</v>
       </c>
       <c r="C15" t="n">
+        <v>78</v>
+      </c>
+      <c r="D15" t="n">
         <v>8</v>
       </c>
-      <c r="D15" t="n">
-        <v>78</v>
-      </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
@@ -865,13 +865,13 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.09302325581395349</v>
+        <v>0.9069767441860465</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1702127659574468</v>
+        <v>0.951219512195122</v>
       </c>
     </row>
     <row r="16">
@@ -882,11 +882,11 @@
         <v>73</v>
       </c>
       <c r="C16" t="n">
+        <v>65</v>
+      </c>
+      <c r="D16" t="n">
         <v>8</v>
       </c>
-      <c r="D16" t="n">
-        <v>65</v>
-      </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
@@ -894,13 +894,13 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1095890410958904</v>
+        <v>0.8904109589041096</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1975308641975309</v>
+        <v>0.9420289855072463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>